<commit_message>
add phenology data and code to process 2020
</commit_message>
<xml_diff>
--- a/data-raw/phen/rd_20200611-phen.xlsx
+++ b/data-raw/phen/rd_20200611-phen.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="19">
   <si>
     <t>date</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>V</t>
+  </si>
+  <si>
+    <t>funleaves_nu</t>
   </si>
 </sst>
 </file>
@@ -475,7 +478,7 @@
   <dimension ref="A1:Q47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -569,7 +572,9 @@
       <c r="H6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="9"/>
+      <c r="I6" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>

</xml_diff>